<commit_message>
added new rsunflo::design to export R experimental design format to websim simulator format. corrected time as a date instead of JDN in rsunflo::shape.
</commit_message>
<xml_diff>
--- a/inst/doc/parameterization.xlsx
+++ b/inst/doc/parameterization.xlsx
@@ -12,14 +12,14 @@
     <sheet name="sunflo_simple" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sunflo!$A$1:$M$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sunflo!$A$1:$M$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="286">
   <si>
     <t>categorie.fr</t>
   </si>
@@ -325,6 +325,12 @@
   </si>
   <si>
     <t>zSemis</t>
+  </si>
+  <si>
+    <t>semis_profondeur</t>
+  </si>
+  <si>
+    <t>crop_sowing_depth</t>
   </si>
   <si>
     <t>Profondeur de semis</t>
@@ -920,8 +926,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FFCC99"/>
-        <bgColor rgb="00C0C0C0"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor rgb="FFC0C0C0"/>
       </patternFill>
     </fill>
   </fills>
@@ -960,20 +966,33 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
       <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -987,10 +1006,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
@@ -998,26 +1013,25 @@
   </sheetPr>
   <dimension ref="A1:M102"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="true" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
-      <pane activePane="bottomLeft" topLeftCell="A47" xSplit="0" ySplit="1"/>
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="F58" activeCellId="0" pane="bottomLeft" sqref="F58"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F15" activeCellId="0" pane="topLeft" sqref="F15"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.62352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.243137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.921568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5372549019608"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8078431372549"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="90.6588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.2078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8117647058824"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="15.8823529411765"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.5647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.62244897959184"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.6122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1377551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5408163265306"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8061224489796"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="90.6581632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.2091836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="15.8826530612245"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="11.8061224489796"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1" s="2">
@@ -1765,11 +1779,17 @@
       <c r="D26" s="0" t="s">
         <v>101</v>
       </c>
+      <c r="E26" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>103</v>
+      </c>
       <c r="G26" s="1" t="n">
         <v>30</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>40</v>
@@ -1780,19 +1800,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="G27" s="1" t="n">
         <v>-25</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I27" s="4"/>
       <c r="L27" s="0" t="n">
@@ -1801,19 +1821,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="G28" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I28" s="4"/>
       <c r="L28" s="0" t="n">
@@ -1822,19 +1842,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="G29" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I29" s="4"/>
       <c r="L29" s="0" t="n">
@@ -1843,22 +1863,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="G30" s="1" t="n">
         <v>350</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L30" s="0" t="n">
         <v>0</v>
@@ -1866,22 +1886,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G31" s="1" t="n">
         <v>86.2</v>
       </c>
       <c r="H31" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="I31" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>113</v>
       </c>
       <c r="L31" s="0" t="n">
         <v>0</v>
@@ -1889,22 +1909,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L32" s="0" t="n">
         <v>0</v>
@@ -1912,19 +1932,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="G33" s="1" t="n">
         <v>4.5</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I33" s="4"/>
       <c r="L33" s="0" t="n">
@@ -1933,22 +1953,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="G34" s="1" t="n">
         <v>0.015</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L34" s="0" t="n">
         <v>0</v>
@@ -1956,22 +1976,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="G35" s="1" t="n">
         <v>3</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L35" s="0" t="n">
         <v>0</v>
@@ -1979,22 +1999,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="G36" s="1" t="n">
         <v>400</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L36" s="0" t="n">
         <v>0</v>
@@ -2002,19 +2022,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="G37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="I37" s="4"/>
       <c r="L37" s="0" t="n">
@@ -2023,22 +2043,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G38" s="1" t="n">
         <v>153</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L38" s="0" t="n">
         <v>0</v>
@@ -2046,22 +2066,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G39" s="1" t="n">
         <v>851.33</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L39" s="0" t="n">
         <v>0</v>
@@ -2069,22 +2089,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="G40" s="1" t="n">
         <v>-0.03783</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L40" s="0" t="n">
         <v>0</v>
@@ -2092,22 +2112,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="G41" s="1" t="n">
         <v>0.78469</v>
       </c>
       <c r="H41" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="L41" s="0" t="n">
         <v>0</v>
@@ -2115,19 +2135,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="G42" s="1" t="n">
         <v>0.01379</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I42" s="4"/>
       <c r="L42" s="0" t="n">
@@ -2136,22 +2156,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="G43" s="1" t="n">
         <v>71.43</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L43" s="0" t="n">
         <v>0</v>
@@ -2159,22 +2179,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G44" s="1" t="n">
         <v>16.34</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L44" s="0" t="n">
         <v>0</v>
@@ -2182,13 +2202,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I45" s="4"/>
       <c r="L45" s="0" t="n">
@@ -2197,13 +2217,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="I46" s="4"/>
       <c r="L46" s="0" t="n">
@@ -2212,13 +2232,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="I47" s="4"/>
       <c r="L47" s="0" t="n">
@@ -2227,13 +2247,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="I48" s="4"/>
       <c r="L48" s="0" t="n">
@@ -2242,13 +2262,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="I49" s="4"/>
       <c r="L49" s="0" t="n">
@@ -2257,22 +2277,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="50">
       <c r="A50" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="I50" s="4"/>
       <c r="L50" s="0" t="n">
@@ -2281,25 +2301,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="51">
       <c r="A51" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L51" s="0" t="n">
         <v>1</v>
@@ -2307,25 +2327,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="52">
       <c r="A52" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E52" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="I52" s="4" t="s">
         <v>161</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>162</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="I52" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="L52" s="0" t="n">
         <v>1</v>
@@ -2333,22 +2353,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="53">
       <c r="A53" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="I53" s="4"/>
       <c r="L53" s="0" t="n">
@@ -2357,22 +2377,22 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="54">
       <c r="A54" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I54" s="4"/>
       <c r="L54" s="0" t="n">
@@ -2381,16 +2401,16 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>40</v>
@@ -2404,22 +2424,22 @@
         <v>13</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L56" s="0" t="n">
         <v>1</v>
@@ -2430,22 +2450,22 @@
         <v>13</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E57" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>185</v>
+      </c>
+      <c r="I57" s="4" t="s">
         <v>181</v>
-      </c>
-      <c r="F57" s="0" t="s">
-        <v>182</v>
-      </c>
-      <c r="H57" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>179</v>
       </c>
       <c r="L57" s="0" t="n">
         <v>1</v>
@@ -2456,13 +2476,13 @@
         <v>13</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="I58" s="4"/>
       <c r="L58" s="0" t="n">
@@ -2474,22 +2494,22 @@
         <v>13</v>
       </c>
       <c r="C59" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D59" s="0" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L59" s="0" t="n">
         <v>1</v>
@@ -2500,22 +2520,22 @@
         <v>13</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L60" s="0" t="n">
         <v>1</v>
@@ -2526,22 +2546,22 @@
         <v>13</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L61" s="0" t="n">
         <v>1</v>
@@ -2552,22 +2572,22 @@
         <v>13</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="L62" s="0" t="n">
         <v>1</v>
@@ -2578,19 +2598,19 @@
         <v>13</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I63" s="4" t="s">
         <v>40</v>
@@ -2604,22 +2624,22 @@
         <v>13</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="L64" s="0" t="n">
         <v>1</v>
@@ -2630,22 +2650,22 @@
         <v>13</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="L65" s="0" t="n">
         <v>1</v>
@@ -2653,25 +2673,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="66">
       <c r="A66" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="I66" s="4"/>
       <c r="L66" s="0" t="n">
@@ -2680,25 +2700,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="67">
       <c r="A67" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="I67" s="4"/>
       <c r="L67" s="0" t="n">
@@ -2707,28 +2727,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="68">
       <c r="A68" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L68" s="0" t="n">
         <v>1</v>
@@ -2736,28 +2756,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="69">
       <c r="A69" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="L69" s="0" t="n">
         <v>1</v>
@@ -2765,28 +2785,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="70">
       <c r="A70" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L70" s="0" t="n">
         <v>1</v>
@@ -2794,28 +2814,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="71">
       <c r="A71" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L71" s="0" t="n">
         <v>1</v>
@@ -2823,28 +2843,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="72">
       <c r="A72" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="F72" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L72" s="0" t="n">
         <v>1</v>
@@ -2852,28 +2872,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="73">
       <c r="A73" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C73" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L73" s="0" t="n">
         <v>1</v>
@@ -2881,25 +2901,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="74">
       <c r="A74" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C74" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I74" s="4"/>
       <c r="L74" s="0" t="n">
@@ -2908,25 +2928,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="75">
       <c r="A75" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F75" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="L75" s="0" t="n">
         <v>1</v>
@@ -2934,25 +2954,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F76" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I76" s="4"/>
       <c r="L76" s="0" t="n">
@@ -2961,28 +2981,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="77">
       <c r="A77" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="F77" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="L77" s="0" t="n">
         <v>1</v>
@@ -2990,25 +3010,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="78">
       <c r="A78" s="0" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="F78" s="0" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="I78" s="4"/>
       <c r="L78" s="0" t="n">
@@ -3017,13 +3037,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="I79" s="4"/>
       <c r="L79" s="0" t="n">
@@ -3032,13 +3052,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C80" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="I80" s="4"/>
       <c r="L80" s="0" t="n">
@@ -3047,13 +3067,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C81" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I81" s="4"/>
       <c r="L81" s="0" t="n">
@@ -3062,13 +3082,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C82" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="I82" s="4"/>
       <c r="L82" s="0" t="n">
@@ -3077,13 +3097,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C83" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="I83" s="4"/>
       <c r="L83" s="0" t="n">
@@ -3092,13 +3112,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C84" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="I84" s="4"/>
       <c r="L84" s="0" t="n">
@@ -3107,13 +3127,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C85" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="I85" s="4"/>
       <c r="L85" s="0" t="n">
@@ -3122,13 +3142,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="I86" s="4"/>
       <c r="L86" s="0" t="n">
@@ -3137,13 +3157,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C87" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="I87" s="4"/>
       <c r="L87" s="0" t="n">
@@ -3152,13 +3172,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C88" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I88" s="4"/>
       <c r="L88" s="0" t="n">
@@ -3167,13 +3187,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C89" s="0" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="I89" s="4"/>
       <c r="L89" s="0" t="n">
@@ -3182,13 +3202,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C90" s="0" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="I90" s="4"/>
       <c r="L90" s="0" t="n">
@@ -3197,19 +3217,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="91">
       <c r="A91" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C91" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="F91" s="0" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="I91" s="4"/>
       <c r="L91" s="0" t="n">
@@ -3218,13 +3238,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C92" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="I92" s="4"/>
       <c r="L92" s="0" t="n">
@@ -3233,13 +3253,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C93" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="I93" s="4"/>
       <c r="L93" s="0" t="n">
@@ -3248,13 +3268,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C94" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D94" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I94" s="4"/>
       <c r="L94" s="0" t="n">
@@ -3263,13 +3283,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C95" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="I95" s="4"/>
       <c r="L95" s="0" t="n">
@@ -3278,13 +3298,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C96" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="I96" s="4"/>
       <c r="L96" s="0" t="n">
@@ -3293,13 +3313,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C97" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="I97" s="4"/>
       <c r="L97" s="0" t="n">
@@ -3308,13 +3328,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C98" s="0" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="I98" s="4"/>
       <c r="L98" s="0" t="n">
@@ -3323,13 +3343,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C99" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="I99" s="4"/>
       <c r="L99" s="0" t="n">
@@ -3338,13 +3358,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C100" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="I100" s="4"/>
       <c r="L100" s="0" t="n">
@@ -3353,13 +3373,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C101" s="0" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="L101" s="0" t="n">
         <v>0</v>
@@ -3367,26 +3387,25 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="F102" s="0" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="H102" s="0" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="L102" s="0" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M102"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
@@ -3394,7 +3413,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3405,12 +3423,13 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6377551020408"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added the manual for a quick sunflo use in doc section
</commit_message>
<xml_diff>
--- a/inst/doc/parameterization.xlsx
+++ b/inst/doc/parameterization.xlsx
@@ -12,6 +12,7 @@
     <sheet name="sunflo_simple" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sunflo!$A$1:$M$102</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">sunflo!$A$1:$M$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -39,15 +40,15 @@
     <t>port.rsunflo.en</t>
   </si>
   <si>
+    <t>label.fr</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
-    <t>label.fr</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
     <t>dimension</t>
   </si>
   <si>
@@ -75,10 +76,10 @@
     <t>file</t>
   </si>
   <si>
+    <t>Nom du fichier climatique</t>
+  </si>
+  <si>
     <t>AUZ_2006.txt</t>
-  </si>
-  <si>
-    <t>Nom du fichier climatique</t>
   </si>
   <si>
     <t>Conduite</t>
@@ -1006,18 +1007,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+  <sheetPr filterMode="true">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M102"/>
+  <dimension ref="1:102"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F15" activeCellId="0" pane="topLeft" sqref="F15"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="F56" activeCellId="0" pane="topLeft" sqref="F56:H65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5816326530612"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.62244897959184"/>
@@ -1025,9 +1030,9 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.25"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1377551020408"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.5408163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.8061224489796"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="90.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="21.2091836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="90.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="21.2091836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.8061224489796"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8061224489796"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="15.8826530612245"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.5612244897959"/>
@@ -1053,13 +1058,13 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
@@ -1074,6 +1079,7 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="AMJ1" s="0"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
@@ -1091,13 +1097,13 @@
       <c r="F2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4"/>
       <c r="L2" s="0" t="n">
         <v>1</v>
       </c>
@@ -1118,14 +1124,14 @@
       <c r="F3" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L3" s="0" t="n">
         <v>1</v>
@@ -1147,20 +1153,20 @@
       <c r="F4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="0" t="s">
+      <c r="G4" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="I4" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="L4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
         <v>20</v>
       </c>
@@ -1176,20 +1182,20 @@
       <c r="F5" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="0" t="s">
+      <c r="G5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="I5" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="L5" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
         <v>20</v>
       </c>
@@ -1205,14 +1211,14 @@
       <c r="F6" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="G6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L6" s="0" t="n">
         <v>0</v>
@@ -1234,14 +1240,14 @@
       <c r="F7" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="G7" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L7" s="0" t="n">
         <v>1</v>
@@ -1263,14 +1269,14 @@
       <c r="F8" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="0" t="s">
+      <c r="G8" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L8" s="0" t="n">
         <v>1</v>
@@ -1292,20 +1298,20 @@
       <c r="F9" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="0" t="s">
+      <c r="G9" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="I9" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="L9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="10">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="10">
       <c r="A10" s="0" t="s">
         <v>20</v>
       </c>
@@ -1321,20 +1327,20 @@
       <c r="F10" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="0" t="s">
+      <c r="G10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="I10" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="L10" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="11">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="11">
       <c r="A11" s="0" t="s">
         <v>20</v>
       </c>
@@ -1350,20 +1356,20 @@
       <c r="F11" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="0" t="s">
+      <c r="G11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="H11" s="4" t="s">
         <v>40</v>
       </c>
+      <c r="I11" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="L11" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>20</v>
       </c>
@@ -1379,14 +1385,14 @@
       <c r="F12" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="0" t="s">
+      <c r="G12" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="H12" s="4" t="s">
         <v>40</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="L12" s="0" t="n">
         <v>0</v>
@@ -1408,14 +1414,14 @@
       <c r="F13" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="5" t="n">
         <v>41275</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L13" s="0" t="n">
         <v>1</v>
@@ -1437,20 +1443,20 @@
       <c r="F14" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="5" t="n">
         <v>41275</v>
       </c>
-      <c r="H14" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L14" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="15">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="15">
       <c r="A15" s="0" t="s">
         <v>20</v>
       </c>
@@ -1466,20 +1472,20 @@
       <c r="F15" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15" s="5" t="n">
         <v>41275</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L15" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="16">
       <c r="A16" s="0" t="s">
         <v>20</v>
       </c>
@@ -1495,14 +1501,14 @@
       <c r="F16" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="5" t="n">
         <v>41275</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L16" s="0" t="n">
         <v>0</v>
@@ -1524,14 +1530,14 @@
       <c r="F17" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="5" t="n">
         <v>41275</v>
-      </c>
-      <c r="H17" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L17" s="0" t="n">
         <v>1</v>
@@ -1553,14 +1559,14 @@
       <c r="F18" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="5" t="n">
         <v>41275</v>
-      </c>
-      <c r="H18" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L18" s="0" t="n">
         <v>1</v>
@@ -1582,20 +1588,20 @@
       <c r="F19" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="5" t="n">
         <v>41275</v>
       </c>
-      <c r="H19" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L19" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="20">
       <c r="A20" s="0" t="s">
         <v>20</v>
       </c>
@@ -1611,20 +1617,20 @@
       <c r="F20" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="5" t="n">
         <v>41275</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L20" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="21">
       <c r="A21" s="0" t="s">
         <v>20</v>
       </c>
@@ -1640,20 +1646,20 @@
       <c r="F21" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="5" t="n">
         <v>41275</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L21" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="22">
       <c r="A22" s="0" t="s">
         <v>20</v>
       </c>
@@ -1669,14 +1675,14 @@
       <c r="F22" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I22" s="5" t="n">
         <v>41275</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L22" s="0" t="n">
         <v>0</v>
@@ -1698,14 +1704,14 @@
       <c r="F23" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="G23" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="I23" s="1" t="n">
         <v>6.8</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="L23" s="0" t="n">
         <v>1</v>
@@ -1727,14 +1733,14 @@
       <c r="F24" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="G24" s="6" t="n">
+      <c r="G24" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I24" s="6" t="n">
         <v>41509</v>
-      </c>
-      <c r="H24" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="L24" s="0" t="n">
         <v>1</v>
@@ -1756,20 +1762,20 @@
       <c r="F25" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="G25" s="6" t="n">
+      <c r="G25" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I25" s="6" t="n">
         <v>41380</v>
       </c>
-      <c r="H25" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>60</v>
-      </c>
       <c r="L25" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="26">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="26">
       <c r="A26" s="0" t="s">
         <v>20</v>
       </c>
@@ -1785,20 +1791,20 @@
       <c r="F26" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="H26" s="0" t="s">
-        <v>104</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="L26" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="27">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="27">
       <c r="A27" s="0" t="s">
         <v>105</v>
       </c>
@@ -1808,18 +1814,18 @@
       <c r="D27" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="G27" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="1" t="n">
         <v>-25</v>
       </c>
-      <c r="H27" s="0" t="s">
-        <v>108</v>
-      </c>
-      <c r="I27" s="4"/>
       <c r="L27" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="28">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="28">
       <c r="A28" s="0" t="s">
         <v>105</v>
       </c>
@@ -1829,18 +1835,18 @@
       <c r="D28" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="G28" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="H28" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="I28" s="4"/>
       <c r="L28" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="29">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="29">
       <c r="A29" s="0" t="s">
         <v>105</v>
       </c>
@@ -1850,18 +1856,18 @@
       <c r="D29" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="G29" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="H29" s="0" t="s">
-        <v>112</v>
-      </c>
-      <c r="I29" s="4"/>
       <c r="L29" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="30">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="30">
       <c r="A30" s="0" t="s">
         <v>105</v>
       </c>
@@ -1871,20 +1877,20 @@
       <c r="D30" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="G30" s="1" t="n">
+      <c r="G30" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I30" s="1" t="n">
         <v>350</v>
       </c>
-      <c r="H30" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L30" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="31">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="31">
       <c r="A31" s="0" t="s">
         <v>105</v>
       </c>
@@ -1894,20 +1900,20 @@
       <c r="D31" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="G31" s="1" t="n">
+      <c r="G31" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I31" s="1" t="n">
         <v>86.2</v>
       </c>
-      <c r="H31" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L31" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="32">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="32">
       <c r="A32" s="0" t="s">
         <v>105</v>
       </c>
@@ -1917,20 +1923,20 @@
       <c r="D32" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="G32" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H32" s="0" t="s">
+      <c r="G32" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="H32" s="4" t="s">
         <v>120</v>
       </c>
+      <c r="I32" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="L32" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="33">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="33">
       <c r="A33" s="0" t="s">
         <v>105</v>
       </c>
@@ -1940,18 +1946,18 @@
       <c r="D33" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="G33" s="1" t="n">
+      <c r="G33" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="1" t="n">
         <v>4.5</v>
       </c>
-      <c r="H33" s="0" t="s">
-        <v>122</v>
-      </c>
-      <c r="I33" s="4"/>
       <c r="L33" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="34">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="34">
       <c r="A34" s="0" t="s">
         <v>105</v>
       </c>
@@ -1961,20 +1967,20 @@
       <c r="D34" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="G34" s="1" t="n">
+      <c r="G34" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I34" s="1" t="n">
         <v>0.015</v>
       </c>
-      <c r="H34" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="L34" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="35">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="35">
       <c r="A35" s="0" t="s">
         <v>105</v>
       </c>
@@ -1984,20 +1990,20 @@
       <c r="D35" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="G35" s="1" t="n">
+      <c r="G35" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="I35" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="H35" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="L35" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="36">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="36">
       <c r="A36" s="0" t="s">
         <v>105</v>
       </c>
@@ -2007,20 +2013,20 @@
       <c r="D36" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="G36" s="1" t="n">
+      <c r="G36" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I36" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="H36" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L36" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="37">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="37">
       <c r="A37" s="0" t="s">
         <v>105</v>
       </c>
@@ -2030,18 +2036,18 @@
       <c r="D37" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="G37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" s="0" t="s">
+      <c r="G37" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="I37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="L37" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="38">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="38">
       <c r="A38" s="0" t="s">
         <v>105</v>
       </c>
@@ -2051,20 +2057,20 @@
       <c r="D38" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="G38" s="1" t="n">
+      <c r="G38" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I38" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="H38" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L38" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="39">
       <c r="A39" s="0" t="s">
         <v>105</v>
       </c>
@@ -2074,20 +2080,20 @@
       <c r="D39" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="G39" s="1" t="n">
+      <c r="G39" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I39" s="1" t="n">
         <v>851.33</v>
       </c>
-      <c r="H39" s="0" t="s">
-        <v>134</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L39" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="40">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="40">
       <c r="A40" s="0" t="s">
         <v>105</v>
       </c>
@@ -2097,20 +2103,20 @@
       <c r="D40" s="0" t="s">
         <v>135</v>
       </c>
-      <c r="G40" s="1" t="n">
+      <c r="G40" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" s="1" t="n">
         <v>-0.03783</v>
       </c>
-      <c r="H40" s="0" t="s">
-        <v>136</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="L40" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="41">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="41">
       <c r="A41" s="0" t="s">
         <v>105</v>
       </c>
@@ -2120,20 +2126,20 @@
       <c r="D41" s="0" t="s">
         <v>138</v>
       </c>
-      <c r="G41" s="1" t="n">
+      <c r="G41" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="I41" s="1" t="n">
         <v>0.78469</v>
       </c>
-      <c r="H41" s="0" t="s">
-        <v>139</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>137</v>
-      </c>
       <c r="L41" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="42">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="42">
       <c r="A42" s="0" t="s">
         <v>105</v>
       </c>
@@ -2143,18 +2149,18 @@
       <c r="D42" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="G42" s="1" t="n">
+      <c r="G42" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="H42" s="4"/>
+      <c r="I42" s="1" t="n">
         <v>0.01379</v>
       </c>
-      <c r="H42" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="I42" s="4"/>
       <c r="L42" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="43">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="43">
       <c r="A43" s="0" t="s">
         <v>105</v>
       </c>
@@ -2164,20 +2170,20 @@
       <c r="D43" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="G43" s="1" t="n">
+      <c r="G43" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I43" s="1" t="n">
         <v>71.43</v>
       </c>
-      <c r="H43" s="0" t="s">
-        <v>143</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L43" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="44">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="44">
       <c r="A44" s="0" t="s">
         <v>105</v>
       </c>
@@ -2187,20 +2193,20 @@
       <c r="D44" s="0" t="s">
         <v>144</v>
       </c>
-      <c r="G44" s="1" t="n">
+      <c r="G44" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I44" s="1" t="n">
         <v>16.34</v>
       </c>
-      <c r="H44" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>115</v>
-      </c>
       <c r="L44" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="45">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="45">
       <c r="A45" s="0" t="s">
         <v>105</v>
       </c>
@@ -2210,12 +2216,12 @@
       <c r="D45" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="I45" s="4"/>
+      <c r="H45" s="4"/>
       <c r="L45" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.2" outlineLevel="0" r="46">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="12.2" outlineLevel="0" r="46">
       <c r="A46" s="0" t="s">
         <v>105</v>
       </c>
@@ -2225,12 +2231,12 @@
       <c r="D46" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="I46" s="4"/>
+      <c r="H46" s="4"/>
       <c r="L46" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="47">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="47">
       <c r="A47" s="0" t="s">
         <v>105</v>
       </c>
@@ -2240,12 +2246,12 @@
       <c r="D47" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="I47" s="4"/>
+      <c r="H47" s="4"/>
       <c r="L47" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="48">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="48">
       <c r="A48" s="0" t="s">
         <v>105</v>
       </c>
@@ -2255,12 +2261,12 @@
       <c r="D48" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="I48" s="4"/>
+      <c r="H48" s="4"/>
       <c r="L48" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="49">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="49">
       <c r="A49" s="0" t="s">
         <v>105</v>
       </c>
@@ -2270,7 +2276,7 @@
       <c r="D49" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="I49" s="4"/>
+      <c r="H49" s="4"/>
       <c r="L49" s="0" t="n">
         <v>0</v>
       </c>
@@ -2291,10 +2297,10 @@
       <c r="F50" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="H50" s="0" t="s">
+      <c r="G50" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="I50" s="4"/>
+      <c r="H50" s="4"/>
       <c r="L50" s="0" t="n">
         <v>1</v>
       </c>
@@ -2315,10 +2321,10 @@
       <c r="F51" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="H51" s="0" t="s">
+      <c r="G51" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="H51" s="4" t="s">
         <v>161</v>
       </c>
       <c r="L51" s="0" t="n">
@@ -2341,10 +2347,10 @@
       <c r="F52" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="H52" s="0" t="s">
+      <c r="G52" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="I52" s="4" t="s">
+      <c r="H52" s="4" t="s">
         <v>161</v>
       </c>
       <c r="L52" s="0" t="n">
@@ -2367,10 +2373,10 @@
       <c r="F53" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="H53" s="0" t="s">
+      <c r="G53" s="0" t="s">
         <v>169</v>
       </c>
-      <c r="I53" s="4"/>
+      <c r="H53" s="4"/>
       <c r="L53" s="0" t="n">
         <v>1</v>
       </c>
@@ -2391,15 +2397,15 @@
       <c r="F54" s="0" t="s">
         <v>172</v>
       </c>
-      <c r="H54" s="0" t="s">
+      <c r="G54" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="I54" s="4"/>
+      <c r="H54" s="4"/>
       <c r="L54" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="55">
       <c r="A55" s="0" t="s">
         <v>151</v>
       </c>
@@ -2409,10 +2415,10 @@
       <c r="D55" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="H55" s="0" t="s">
+      <c r="G55" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="I55" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>40</v>
       </c>
       <c r="L55" s="0" t="n">
@@ -2435,10 +2441,10 @@
       <c r="F56" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="H56" s="0" t="s">
+      <c r="G56" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="I56" s="4" t="s">
+      <c r="H56" s="4" t="s">
         <v>181</v>
       </c>
       <c r="L56" s="0" t="n">
@@ -2461,17 +2467,17 @@
       <c r="F57" s="0" t="s">
         <v>184</v>
       </c>
-      <c r="H57" s="0" t="s">
+      <c r="G57" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="I57" s="4" t="s">
+      <c r="H57" s="4" t="s">
         <v>181</v>
       </c>
       <c r="L57" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="58">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="58">
       <c r="A58" s="0" t="s">
         <v>13</v>
       </c>
@@ -2481,10 +2487,10 @@
       <c r="D58" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="H58" s="0" t="s">
+      <c r="G58" s="0" t="s">
         <v>187</v>
       </c>
-      <c r="I58" s="4"/>
+      <c r="H58" s="4"/>
       <c r="L58" s="0" t="n">
         <v>0</v>
       </c>
@@ -2505,10 +2511,10 @@
       <c r="F59" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="H59" s="0" t="s">
+      <c r="G59" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="I59" s="4" t="s">
+      <c r="H59" s="4" t="s">
         <v>161</v>
       </c>
       <c r="L59" s="0" t="n">
@@ -2531,10 +2537,10 @@
       <c r="F60" s="0" t="s">
         <v>194</v>
       </c>
-      <c r="H60" s="0" t="s">
+      <c r="G60" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="I60" s="4" t="s">
+      <c r="H60" s="4" t="s">
         <v>161</v>
       </c>
       <c r="L60" s="0" t="n">
@@ -2557,10 +2563,10 @@
       <c r="F61" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="H61" s="0" t="s">
+      <c r="G61" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="I61" s="4" t="s">
+      <c r="H61" s="4" t="s">
         <v>161</v>
       </c>
       <c r="L61" s="0" t="n">
@@ -2583,10 +2589,10 @@
       <c r="F62" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="H62" s="0" t="s">
+      <c r="G62" s="0" t="s">
         <v>203</v>
       </c>
-      <c r="I62" s="4" t="s">
+      <c r="H62" s="4" t="s">
         <v>161</v>
       </c>
       <c r="L62" s="0" t="n">
@@ -2609,10 +2615,10 @@
       <c r="F63" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="H63" s="0" t="s">
+      <c r="G63" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="I63" s="4" t="s">
+      <c r="H63" s="4" t="s">
         <v>40</v>
       </c>
       <c r="L63" s="0" t="n">
@@ -2635,10 +2641,10 @@
       <c r="F64" s="0" t="s">
         <v>209</v>
       </c>
-      <c r="H64" s="0" t="s">
+      <c r="G64" s="0" t="s">
         <v>210</v>
       </c>
-      <c r="I64" s="4" t="s">
+      <c r="H64" s="4" t="s">
         <v>211</v>
       </c>
       <c r="L64" s="0" t="n">
@@ -2661,10 +2667,10 @@
       <c r="F65" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="H65" s="0" t="s">
+      <c r="G65" s="0" t="s">
         <v>215</v>
       </c>
-      <c r="I65" s="4" t="s">
+      <c r="H65" s="4" t="s">
         <v>216</v>
       </c>
       <c r="L65" s="0" t="n">
@@ -2687,13 +2693,13 @@
       <c r="E66" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="F66" s="0" t="s">
+      <c r="F66" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="H66" s="0" t="s">
+      <c r="G66" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="I66" s="4"/>
+      <c r="H66" s="4"/>
       <c r="L66" s="0" t="n">
         <v>1</v>
       </c>
@@ -2717,10 +2723,10 @@
       <c r="F67" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="H67" s="0" t="s">
+      <c r="G67" s="0" t="s">
         <v>224</v>
       </c>
-      <c r="I67" s="4"/>
+      <c r="H67" s="4"/>
       <c r="L67" s="0" t="n">
         <v>1</v>
       </c>
@@ -2744,10 +2750,10 @@
       <c r="F68" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="H68" s="0" t="s">
+      <c r="G68" s="0" t="s">
         <v>227</v>
       </c>
-      <c r="I68" s="4" t="s">
+      <c r="H68" s="4" t="s">
         <v>137</v>
       </c>
       <c r="L68" s="0" t="n">
@@ -2773,10 +2779,10 @@
       <c r="F69" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="H69" s="0" t="s">
+      <c r="G69" s="0" t="s">
         <v>230</v>
       </c>
-      <c r="I69" s="4" t="s">
+      <c r="H69" s="4" t="s">
         <v>231</v>
       </c>
       <c r="L69" s="0" t="n">
@@ -2802,10 +2808,10 @@
       <c r="F70" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="H70" s="0" t="s">
+      <c r="G70" s="0" t="s">
         <v>234</v>
       </c>
-      <c r="I70" s="4" t="s">
+      <c r="H70" s="4" t="s">
         <v>115</v>
       </c>
       <c r="L70" s="0" t="n">
@@ -2831,10 +2837,10 @@
       <c r="F71" s="0" t="s">
         <v>236</v>
       </c>
-      <c r="H71" s="0" t="s">
+      <c r="G71" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="I71" s="4" t="s">
+      <c r="H71" s="4" t="s">
         <v>115</v>
       </c>
       <c r="L71" s="0" t="n">
@@ -2860,10 +2866,10 @@
       <c r="F72" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="H72" s="0" t="s">
+      <c r="G72" s="0" t="s">
         <v>240</v>
       </c>
-      <c r="I72" s="4" t="s">
+      <c r="H72" s="4" t="s">
         <v>115</v>
       </c>
       <c r="L72" s="0" t="n">
@@ -2889,10 +2895,10 @@
       <c r="F73" s="0" t="s">
         <v>242</v>
       </c>
-      <c r="H73" s="0" t="s">
+      <c r="G73" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="I73" s="4" t="s">
+      <c r="H73" s="4" t="s">
         <v>115</v>
       </c>
       <c r="L73" s="0" t="n">
@@ -2918,10 +2924,10 @@
       <c r="F74" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="H74" s="0" t="s">
+      <c r="G74" s="0" t="s">
         <v>246</v>
       </c>
-      <c r="I74" s="4"/>
+      <c r="H74" s="4"/>
       <c r="L74" s="0" t="n">
         <v>1</v>
       </c>
@@ -2945,14 +2951,14 @@
       <c r="F75" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="H75" s="0" t="s">
+      <c r="G75" s="0" t="s">
         <v>249</v>
       </c>
       <c r="L75" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="76">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="76">
       <c r="A76" s="0" t="s">
         <v>217</v>
       </c>
@@ -2971,10 +2977,10 @@
       <c r="F76" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="H76" s="0" t="s">
+      <c r="G76" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="I76" s="4"/>
+      <c r="H76" s="4"/>
       <c r="L76" s="0" t="n">
         <v>0</v>
       </c>
@@ -2998,10 +3004,10 @@
       <c r="F77" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="H77" s="0" t="s">
+      <c r="G77" s="0" t="s">
         <v>254</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="H77" s="4" t="s">
         <v>255</v>
       </c>
       <c r="L77" s="0" t="n">
@@ -3027,15 +3033,15 @@
       <c r="F78" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="H78" s="0" t="s">
+      <c r="G78" s="0" t="s">
         <v>257</v>
       </c>
-      <c r="I78" s="4"/>
+      <c r="H78" s="4"/>
       <c r="L78" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="79">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="79">
       <c r="A79" s="0" t="s">
         <v>105</v>
       </c>
@@ -3045,12 +3051,12 @@
       <c r="D79" s="0" t="s">
         <v>259</v>
       </c>
-      <c r="I79" s="4"/>
+      <c r="H79" s="4"/>
       <c r="L79" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="80">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="80">
       <c r="A80" s="0" t="s">
         <v>105</v>
       </c>
@@ -3060,12 +3066,12 @@
       <c r="D80" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="I80" s="4"/>
+      <c r="H80" s="4"/>
       <c r="L80" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="81">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="81">
       <c r="A81" s="0" t="s">
         <v>105</v>
       </c>
@@ -3075,12 +3081,12 @@
       <c r="D81" s="0" t="s">
         <v>261</v>
       </c>
-      <c r="I81" s="4"/>
+      <c r="H81" s="4"/>
       <c r="L81" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="82">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="82">
       <c r="A82" s="0" t="s">
         <v>105</v>
       </c>
@@ -3090,12 +3096,12 @@
       <c r="D82" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="I82" s="4"/>
+      <c r="H82" s="4"/>
       <c r="L82" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="83">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="83">
       <c r="A83" s="0" t="s">
         <v>105</v>
       </c>
@@ -3105,12 +3111,12 @@
       <c r="D83" s="0" t="s">
         <v>263</v>
       </c>
-      <c r="I83" s="4"/>
+      <c r="H83" s="4"/>
       <c r="L83" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="84">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="84">
       <c r="A84" s="0" t="s">
         <v>105</v>
       </c>
@@ -3120,12 +3126,12 @@
       <c r="D84" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="I84" s="4"/>
+      <c r="H84" s="4"/>
       <c r="L84" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="85">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="85">
       <c r="A85" s="0" t="s">
         <v>105</v>
       </c>
@@ -3135,12 +3141,12 @@
       <c r="D85" s="0" t="s">
         <v>265</v>
       </c>
-      <c r="I85" s="4"/>
+      <c r="H85" s="4"/>
       <c r="L85" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="86">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="86">
       <c r="A86" s="0" t="s">
         <v>105</v>
       </c>
@@ -3150,12 +3156,12 @@
       <c r="D86" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="I86" s="4"/>
+      <c r="H86" s="4"/>
       <c r="L86" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="87">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="87">
       <c r="A87" s="0" t="s">
         <v>105</v>
       </c>
@@ -3165,12 +3171,12 @@
       <c r="D87" s="0" t="s">
         <v>267</v>
       </c>
-      <c r="I87" s="4"/>
+      <c r="H87" s="4"/>
       <c r="L87" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="88">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="88">
       <c r="A88" s="0" t="s">
         <v>105</v>
       </c>
@@ -3180,12 +3186,12 @@
       <c r="D88" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="I88" s="4"/>
+      <c r="H88" s="4"/>
       <c r="L88" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="89">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="89">
       <c r="A89" s="0" t="s">
         <v>105</v>
       </c>
@@ -3195,12 +3201,12 @@
       <c r="D89" s="0" t="s">
         <v>269</v>
       </c>
-      <c r="I89" s="4"/>
+      <c r="H89" s="4"/>
       <c r="L89" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="90">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="90">
       <c r="A90" s="0" t="s">
         <v>105</v>
       </c>
@@ -3210,7 +3216,7 @@
       <c r="D90" s="0" t="s">
         <v>271</v>
       </c>
-      <c r="I90" s="4"/>
+      <c r="H90" s="4"/>
       <c r="L90" s="0" t="n">
         <v>0</v>
       </c>
@@ -3231,12 +3237,12 @@
       <c r="F91" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="I91" s="4"/>
+      <c r="H91" s="4"/>
       <c r="L91" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="92">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="92">
       <c r="A92" s="0" t="s">
         <v>272</v>
       </c>
@@ -3246,12 +3252,12 @@
       <c r="D92" s="0" t="s">
         <v>275</v>
       </c>
-      <c r="I92" s="4"/>
+      <c r="H92" s="4"/>
       <c r="L92" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="93">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="93">
       <c r="A93" s="0" t="s">
         <v>272</v>
       </c>
@@ -3261,12 +3267,12 @@
       <c r="D93" s="0" t="s">
         <v>276</v>
       </c>
-      <c r="I93" s="4"/>
+      <c r="H93" s="4"/>
       <c r="L93" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="94">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="94">
       <c r="A94" s="0" t="s">
         <v>272</v>
       </c>
@@ -3276,12 +3282,12 @@
       <c r="D94" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="I94" s="4"/>
+      <c r="H94" s="4"/>
       <c r="L94" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="95">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="95">
       <c r="A95" s="0" t="s">
         <v>272</v>
       </c>
@@ -3291,12 +3297,12 @@
       <c r="D95" s="0" t="s">
         <v>278</v>
       </c>
-      <c r="I95" s="4"/>
+      <c r="H95" s="4"/>
       <c r="L95" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="96">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="96">
       <c r="A96" s="0" t="s">
         <v>272</v>
       </c>
@@ -3306,12 +3312,12 @@
       <c r="D96" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="I96" s="4"/>
+      <c r="H96" s="4"/>
       <c r="L96" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="97">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="97">
       <c r="A97" s="0" t="s">
         <v>272</v>
       </c>
@@ -3321,12 +3327,12 @@
       <c r="D97" s="0" t="s">
         <v>280</v>
       </c>
-      <c r="I97" s="4"/>
+      <c r="H97" s="4"/>
       <c r="L97" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="98">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="98">
       <c r="A98" s="0" t="s">
         <v>272</v>
       </c>
@@ -3336,12 +3342,12 @@
       <c r="D98" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="I98" s="4"/>
+      <c r="H98" s="4"/>
       <c r="L98" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="99">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="99">
       <c r="A99" s="0" t="s">
         <v>272</v>
       </c>
@@ -3351,12 +3357,12 @@
       <c r="D99" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="I99" s="4"/>
+      <c r="H99" s="4"/>
       <c r="L99" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="100">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="100">
       <c r="A100" s="0" t="s">
         <v>272</v>
       </c>
@@ -3366,12 +3372,12 @@
       <c r="D100" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="I100" s="4"/>
+      <c r="H100" s="4"/>
       <c r="L100" s="0" t="n">
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="13.2" outlineLevel="0" r="101">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="true" ht="13.2" outlineLevel="0" r="101">
       <c r="A101" s="0" t="s">
         <v>272</v>
       </c>
@@ -3385,7 +3391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.2" outlineLevel="0" r="102">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="102">
       <c r="A102" s="0" t="s">
         <v>272</v>
       </c>
@@ -3398,7 +3404,7 @@
       <c r="F102" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="H102" s="0" t="s">
+      <c r="G102" s="0" t="s">
         <v>285</v>
       </c>
       <c r="L102" s="0" t="n">
@@ -3406,6 +3412,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M102">
+    <filterColumn colId="11">
+      <customFilters and="true">
+        <customFilter operator="equal" val="1"/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
@@ -3413,6 +3426,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3424,7 +3438,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="F56:H65 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
added details about simulation templates in user notice
</commit_message>
<xml_diff>
--- a/inst/doc/parameterization.xlsx
+++ b/inst/doc/parameterization.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="2" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="393" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="375" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="sunflo_input" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,6 +22,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">sunflo_input!$A$1:$O$102</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">sunflo_input!$A$1:$O$102</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">sunflo_input!$A$1:$O$102</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">sunflo_input!$A$1:$O$102</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -693,7 +694,7 @@
     <t>crop_emergence</t>
   </si>
   <si>
-    <t>Date de levée (forçage)</t>
+    <t>Date de levée forcée, simulée pour valeur = 01/01</t>
   </si>
   <si>
     <t>rh1</t>
@@ -1573,32 +1574,32 @@
   </numFmts>
   <fonts count="5">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-      <sz val="10"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <charset val="1"/>
-      <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1654,10 +1655,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="2" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -1668,6 +1665,10 @@
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
+      <alignment horizontal="right" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0">
@@ -1705,8 +1706,8 @@
   </sheetPr>
   <dimension ref="1:102"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H9" activeCellId="0" pane="topLeft" sqref="H9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="H53" activeCellId="0" pane="topLeft" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.2"/>
@@ -1722,56 +1723,56 @@
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="55.3826530612245"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2091836734694"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.5969387755102"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.8061224489796"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="12.8061224489796"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="0" width="15.8826530612245"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="13.5612244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="11.8061224489796"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1" s="2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="12.8" outlineLevel="0" r="1" s="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="AMJ1" s="0"/>
@@ -1804,7 +1805,7 @@
       <c r="I2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K2" s="0" t="s">
@@ -1842,7 +1843,7 @@
       <c r="I3" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K3" s="0" t="s">
@@ -1880,7 +1881,7 @@
       <c r="I4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K4" s="0" t="s">
@@ -1918,7 +1919,7 @@
       <c r="I5" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="0" t="s">
@@ -1956,7 +1957,7 @@
       <c r="I6" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K6" s="0" t="s">
@@ -1994,7 +1995,7 @@
       <c r="I7" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K7" s="0" t="s">
@@ -2032,7 +2033,7 @@
       <c r="I8" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="3" t="s">
         <v>47</v>
       </c>
       <c r="K8" s="0" t="s">
@@ -2070,7 +2071,7 @@
       <c r="I9" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="J9" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K9" s="0" t="s">
@@ -2099,16 +2100,16 @@
       <c r="F10" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="3" t="s">
         <v>55</v>
       </c>
       <c r="I10" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K10" s="0" t="s">
@@ -2146,7 +2147,7 @@
       <c r="I11" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="J11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K11" s="0" t="s">
@@ -2184,7 +2185,7 @@
       <c r="I12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="4"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="0" t="s">
         <v>22</v>
       </c>
@@ -2258,7 +2259,7 @@
       <c r="I14" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="3" t="s">
         <v>74</v>
       </c>
       <c r="K14" s="0" t="s">
@@ -2290,10 +2291,10 @@
       <c r="H15" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L15" s="4" t="s">
         <v>81</v>
       </c>
       <c r="N15" s="0" t="n">
@@ -2322,7 +2323,7 @@
       <c r="H16" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="3" t="s">
         <v>86</v>
       </c>
       <c r="K16" s="0" t="s">
@@ -2354,7 +2355,7 @@
       <c r="H17" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N17" s="0" t="n">
@@ -2383,7 +2384,7 @@
       <c r="H18" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J18" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N18" s="0" t="n">
@@ -2412,7 +2413,7 @@
       <c r="H19" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="J19" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N19" s="0" t="n">
@@ -2441,7 +2442,7 @@
       <c r="H20" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N20" s="0" t="n">
@@ -2470,7 +2471,7 @@
       <c r="H21" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N21" s="0" t="n">
@@ -2499,7 +2500,7 @@
       <c r="H22" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="3" t="s">
         <v>108</v>
       </c>
       <c r="N22" s="0" t="n">
@@ -2528,7 +2529,7 @@
       <c r="H23" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="3" t="s">
         <v>117</v>
       </c>
       <c r="N23" s="0" t="n">
@@ -2557,7 +2558,7 @@
       <c r="H24" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J24" s="3" t="s">
         <v>122</v>
       </c>
       <c r="K24" s="0" t="s">
@@ -2583,7 +2584,7 @@
       <c r="H25" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J25" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K25" s="0" t="s">
@@ -2615,7 +2616,7 @@
       <c r="H26" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="J26" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L26" s="5" t="n">
@@ -2647,7 +2648,7 @@
       <c r="H27" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J27" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L27" s="5" t="n">
@@ -2679,10 +2680,10 @@
       <c r="H28" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="J28" s="4" t="s">
+      <c r="J28" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L28" s="1" t="n">
+      <c r="L28" s="4" t="n">
         <v>30</v>
       </c>
       <c r="N28" s="0" t="n">
@@ -2711,10 +2712,10 @@
       <c r="H29" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="J29" s="4" t="s">
+      <c r="J29" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="L29" s="1" t="n">
+      <c r="L29" s="4" t="n">
         <v>6.8</v>
       </c>
       <c r="N29" s="0" t="n">
@@ -2743,7 +2744,7 @@
       <c r="H30" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="J30" s="4" t="s">
+      <c r="J30" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L30" s="6" t="n">
@@ -2775,10 +2776,10 @@
       <c r="H31" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="J31" s="4" t="s">
+      <c r="J31" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L31" s="1" t="n">
+      <c r="L31" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N31" s="0" t="n">
@@ -2807,7 +2808,7 @@
       <c r="H32" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="J32" s="4" t="s">
+      <c r="J32" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L32" s="6" t="n">
@@ -2839,10 +2840,10 @@
       <c r="H33" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="J33" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L33" s="1" t="n">
+      <c r="L33" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N33" s="0" t="n">
@@ -2871,7 +2872,7 @@
       <c r="H34" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="J34" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L34" s="6" t="n">
@@ -2903,10 +2904,10 @@
       <c r="H35" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="J35" s="4" t="s">
+      <c r="J35" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L35" s="1" t="n">
+      <c r="L35" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N35" s="0" t="n">
@@ -2935,7 +2936,7 @@
       <c r="H36" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="J36" s="4" t="s">
+      <c r="J36" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L36" s="6" t="n">
@@ -2967,10 +2968,10 @@
       <c r="H37" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="J37" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="L37" s="1" t="n">
+      <c r="L37" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N37" s="0" t="n">
@@ -2999,7 +3000,7 @@
       <c r="H38" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="J38" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L38" s="6" t="n">
@@ -3031,10 +3032,10 @@
       <c r="H39" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="J39" s="4" t="s">
+      <c r="J39" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L39" s="1" t="n">
+      <c r="L39" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N39" s="0" t="n">
@@ -3063,7 +3064,7 @@
       <c r="H40" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="J40" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L40" s="6" t="n">
@@ -3095,10 +3096,10 @@
       <c r="H41" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="J41" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L41" s="1" t="n">
+      <c r="L41" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N41" s="0" t="n">
@@ -3127,7 +3128,7 @@
       <c r="H42" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="J42" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L42" s="6" t="n">
@@ -3159,10 +3160,10 @@
       <c r="H43" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="J43" s="4" t="s">
+      <c r="J43" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L43" s="1" t="n">
+      <c r="L43" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N43" s="0" t="n">
@@ -3191,7 +3192,7 @@
       <c r="H44" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J44" s="4" t="s">
+      <c r="J44" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L44" s="6" t="n">
@@ -3223,10 +3224,10 @@
       <c r="H45" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="J45" s="4" t="s">
+      <c r="J45" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L45" s="1" t="n">
+      <c r="L45" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N45" s="0" t="n">
@@ -3255,7 +3256,7 @@
       <c r="H46" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J46" s="4" t="s">
+      <c r="J46" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L46" s="6" t="n">
@@ -3287,10 +3288,10 @@
       <c r="H47" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="J47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L47" s="1" t="n">
+      <c r="L47" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N47" s="0" t="n">
@@ -3319,7 +3320,7 @@
       <c r="H48" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="J48" s="4" t="s">
+      <c r="J48" s="3" t="s">
         <v>132</v>
       </c>
       <c r="L48" s="6" t="n">
@@ -3351,10 +3352,10 @@
       <c r="H49" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="J49" s="4" t="s">
+      <c r="J49" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L49" s="1" t="n">
+      <c r="L49" s="4" t="n">
         <v>0</v>
       </c>
       <c r="N49" s="0" t="n">
@@ -3380,7 +3381,7 @@
       <c r="H50" s="0" t="s">
         <v>212</v>
       </c>
-      <c r="J50" s="4" t="s">
+      <c r="J50" s="3" t="s">
         <v>213</v>
       </c>
       <c r="N50" s="0" t="n">
@@ -3435,7 +3436,7 @@
       <c r="H52" s="0" t="s">
         <v>221</v>
       </c>
-      <c r="J52" s="4" t="s">
+      <c r="J52" s="3" t="s">
         <v>132</v>
       </c>
       <c r="N52" s="0" t="n">
@@ -3464,7 +3465,7 @@
       <c r="H53" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="J53" s="4" t="s">
+      <c r="J53" s="3" t="s">
         <v>153</v>
       </c>
       <c r="N53" s="0" t="n">
@@ -3493,7 +3494,7 @@
       <c r="H54" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="J54" s="4" t="s">
+      <c r="J54" s="3" t="s">
         <v>153</v>
       </c>
       <c r="N54" s="0" t="n">
@@ -3522,7 +3523,7 @@
       <c r="H55" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="J55" s="4" t="s">
+      <c r="J55" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N55" s="0" t="n">
@@ -3551,7 +3552,7 @@
       <c r="H56" s="0" t="s">
         <v>237</v>
       </c>
-      <c r="J56" s="4" t="s">
+      <c r="J56" s="3" t="s">
         <v>91</v>
       </c>
       <c r="N56" s="0" t="n">
@@ -3574,10 +3575,10 @@
       <c r="H57" s="0" t="s">
         <v>239</v>
       </c>
-      <c r="J57" s="4" t="s">
+      <c r="J57" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="L57" s="1" t="n">
+      <c r="L57" s="4" t="n">
         <v>300</v>
       </c>
       <c r="N57" s="0" t="n">
@@ -3600,13 +3601,13 @@
       <c r="H58" s="0" t="s">
         <v>243</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="J58" s="3" t="s">
         <v>244</v>
       </c>
       <c r="K58" s="0" t="s">
         <v>245</v>
       </c>
-      <c r="L58" s="1" t="n">
+      <c r="L58" s="4" t="n">
         <v>4.8</v>
       </c>
       <c r="N58" s="0" t="n">
@@ -3629,13 +3630,13 @@
       <c r="H59" s="0" t="s">
         <v>247</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="J59" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K59" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="L59" s="1" t="n">
+      <c r="L59" s="4" t="n">
         <v>86.2</v>
       </c>
       <c r="N59" s="0" t="n">
@@ -3658,13 +3659,13 @@
       <c r="H60" s="0" t="s">
         <v>250</v>
       </c>
-      <c r="J60" s="4" t="s">
+      <c r="J60" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K60" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="L60" s="1" t="n">
+      <c r="L60" s="4" t="n">
         <v>71.43</v>
       </c>
       <c r="N60" s="0" t="n">
@@ -3687,13 +3688,13 @@
       <c r="H61" s="0" t="s">
         <v>253</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="J61" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K61" s="0" t="s">
         <v>251</v>
       </c>
-      <c r="L61" s="1" t="n">
+      <c r="L61" s="4" t="n">
         <v>16.34</v>
       </c>
       <c r="N61" s="0" t="n">
@@ -3716,13 +3717,13 @@
       <c r="H62" s="0" t="s">
         <v>255</v>
       </c>
-      <c r="J62" s="4" t="s">
+      <c r="J62" s="3" t="s">
         <v>86</v>
       </c>
       <c r="K62" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L62" s="1" t="n">
+      <c r="L62" s="4" t="n">
         <v>1800</v>
       </c>
       <c r="N62" s="0" t="n">
@@ -3745,13 +3746,13 @@
       <c r="H63" s="0" t="s">
         <v>258</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="J63" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K63" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L63" s="1" t="n">
+      <c r="L63" s="4" t="n">
         <v>0.1</v>
       </c>
       <c r="N63" s="0" t="n">
@@ -3774,13 +3775,13 @@
       <c r="H64" s="0" t="s">
         <v>260</v>
       </c>
-      <c r="J64" s="4" t="s">
+      <c r="J64" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K64" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L64" s="1" t="n">
+      <c r="L64" s="4" t="n">
         <v>400</v>
       </c>
       <c r="N64" s="0" t="n">
@@ -3803,13 +3804,13 @@
       <c r="H65" s="0" t="s">
         <v>262</v>
       </c>
-      <c r="J65" s="4" t="s">
+      <c r="J65" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K65" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L65" s="1" t="n">
+      <c r="L65" s="4" t="n">
         <v>1</v>
       </c>
       <c r="N65" s="0" t="n">
@@ -3832,13 +3833,13 @@
       <c r="H66" s="0" t="s">
         <v>264</v>
       </c>
-      <c r="J66" s="4" t="s">
+      <c r="J66" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K66" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L66" s="1" t="n">
+      <c r="L66" s="4" t="n">
         <v>153</v>
       </c>
       <c r="N66" s="0" t="n">
@@ -3861,13 +3862,13 @@
       <c r="H67" s="0" t="s">
         <v>266</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="J67" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K67" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L67" s="1" t="n">
+      <c r="L67" s="4" t="n">
         <v>851.33</v>
       </c>
       <c r="N67" s="0" t="n">
@@ -3890,13 +3891,13 @@
       <c r="H68" s="0" t="s">
         <v>268</v>
       </c>
-      <c r="J68" s="4" t="s">
+      <c r="J68" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K68" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L68" s="1" t="n">
+      <c r="L68" s="4" t="n">
         <v>-0.03783</v>
       </c>
       <c r="N68" s="0" t="n">
@@ -3919,13 +3920,13 @@
       <c r="H69" s="0" t="s">
         <v>270</v>
       </c>
-      <c r="J69" s="4" t="s">
+      <c r="J69" s="3" t="s">
         <v>38</v>
       </c>
       <c r="K69" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L69" s="1" t="n">
+      <c r="L69" s="4" t="n">
         <v>0.78469</v>
       </c>
       <c r="N69" s="0" t="n">
@@ -3948,13 +3949,13 @@
       <c r="H70" s="0" t="s">
         <v>272</v>
       </c>
-      <c r="J70" s="4" t="s">
+      <c r="J70" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K70" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L70" s="1" t="n">
+      <c r="L70" s="4" t="n">
         <v>0.01379</v>
       </c>
       <c r="N70" s="0" t="n">
@@ -3977,13 +3978,13 @@
       <c r="H71" s="0" t="s">
         <v>274</v>
       </c>
-      <c r="J71" s="4" t="s">
+      <c r="J71" s="3" t="s">
         <v>275</v>
       </c>
       <c r="K71" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L71" s="1" t="n">
+      <c r="L71" s="4" t="n">
         <v>1</v>
       </c>
       <c r="N71" s="0" t="n">
@@ -4006,13 +4007,13 @@
       <c r="H72" s="0" t="s">
         <v>277</v>
       </c>
-      <c r="J72" s="4" t="s">
+      <c r="J72" s="3" t="s">
         <v>275</v>
       </c>
       <c r="K72" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L72" s="1" t="n">
+      <c r="L72" s="4" t="n">
         <v>4.5</v>
       </c>
       <c r="N72" s="0" t="n">
@@ -4035,13 +4036,13 @@
       <c r="H73" s="0" t="s">
         <v>279</v>
       </c>
-      <c r="J73" s="4" t="s">
+      <c r="J73" s="3" t="s">
         <v>275</v>
       </c>
       <c r="K73" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L73" s="1" t="n">
+      <c r="L73" s="4" t="n">
         <v>0.015</v>
       </c>
       <c r="N73" s="0" t="n">
@@ -4064,13 +4065,13 @@
       <c r="H74" s="0" t="s">
         <v>281</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="J74" s="3" t="s">
         <v>275</v>
       </c>
       <c r="K74" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L74" s="1" t="n">
+      <c r="L74" s="4" t="n">
         <v>3</v>
       </c>
       <c r="N74" s="0" t="n">
@@ -4093,13 +4094,13 @@
       <c r="H75" s="0" t="s">
         <v>283</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="J75" s="3" t="s">
         <v>244</v>
       </c>
       <c r="K75" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L75" s="1" t="n">
+      <c r="L75" s="4" t="n">
         <v>37</v>
       </c>
       <c r="N75" s="0" t="n">
@@ -4119,17 +4120,17 @@
       <c r="E76" s="0" t="s">
         <v>284</v>
       </c>
-      <c r="H76" s="4" t="s">
+      <c r="H76" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="I76" s="4"/>
-      <c r="J76" s="4" t="s">
+      <c r="I76" s="3"/>
+      <c r="J76" s="3" t="s">
         <v>244</v>
       </c>
       <c r="K76" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L76" s="1" t="n">
+      <c r="L76" s="4" t="n">
         <v>20</v>
       </c>
       <c r="N76" s="0" t="n">
@@ -4149,17 +4150,17 @@
       <c r="E77" s="0" t="s">
         <v>286</v>
       </c>
-      <c r="H77" s="4" t="s">
+      <c r="H77" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="I77" s="4"/>
-      <c r="J77" s="4" t="s">
+      <c r="I77" s="3"/>
+      <c r="J77" s="3" t="s">
         <v>244</v>
       </c>
       <c r="K77" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L77" s="1" t="n">
+      <c r="L77" s="4" t="n">
         <v>28</v>
       </c>
       <c r="N77" s="0" t="n">
@@ -4182,13 +4183,13 @@
       <c r="H78" s="0" t="s">
         <v>289</v>
       </c>
-      <c r="J78" s="4" t="s">
+      <c r="J78" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K78" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L78" s="1" t="n">
+      <c r="L78" s="4" t="n">
         <v>-25</v>
       </c>
       <c r="N78" s="0" t="n">
@@ -4211,13 +4212,13 @@
       <c r="H79" s="0" t="s">
         <v>291</v>
       </c>
-      <c r="J79" s="4" t="s">
+      <c r="J79" s="3" t="s">
         <v>21</v>
       </c>
       <c r="K79" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L79" s="1" t="n">
+      <c r="L79" s="4" t="n">
         <v>350</v>
       </c>
       <c r="N79" s="0" t="n">
@@ -4240,13 +4241,13 @@
       <c r="H80" s="0" t="s">
         <v>293</v>
       </c>
-      <c r="J80" s="4" t="s">
+      <c r="J80" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K80" s="0" t="s">
         <v>256</v>
       </c>
-      <c r="L80" s="1" t="n">
+      <c r="L80" s="4" t="n">
         <v>0.1</v>
       </c>
       <c r="N80" s="0" t="n">
@@ -4269,13 +4270,13 @@
       <c r="H81" s="0" t="s">
         <v>296</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="J81" s="3" t="s">
         <v>91</v>
       </c>
       <c r="K81" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="L81" s="1" t="n">
+      <c r="L81" s="4" t="n">
         <v>4.53</v>
       </c>
       <c r="N81" s="0" t="n">
@@ -4298,13 +4299,13 @@
       <c r="H82" s="0" t="s">
         <v>299</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="J82" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K82" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="L82" s="1" t="n">
+      <c r="L82" s="4" t="n">
         <v>0.42</v>
       </c>
       <c r="N82" s="0" t="n">
@@ -4327,13 +4328,13 @@
       <c r="H83" s="0" t="s">
         <v>301</v>
       </c>
-      <c r="J83" s="4" t="s">
+      <c r="J83" s="3" t="s">
         <v>91</v>
       </c>
       <c r="K83" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="L83" s="1" t="n">
+      <c r="L83" s="4" t="n">
         <v>6.49</v>
       </c>
       <c r="N83" s="0" t="n">
@@ -4356,13 +4357,13 @@
       <c r="H84" s="0" t="s">
         <v>303</v>
       </c>
-      <c r="J84" s="4" t="s">
+      <c r="J84" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K84" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="L84" s="1" t="n">
+      <c r="L84" s="4" t="n">
         <v>0.44</v>
       </c>
       <c r="N84" s="0" t="n">
@@ -4385,13 +4386,13 @@
       <c r="H85" s="0" t="s">
         <v>305</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="J85" s="3" t="s">
         <v>306</v>
       </c>
       <c r="K85" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="L85" s="1" t="n">
+      <c r="L85" s="4" t="n">
         <v>75</v>
       </c>
       <c r="N85" s="0" t="n">
@@ -4414,13 +4415,13 @@
       <c r="H86" s="0" t="s">
         <v>308</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="J86" s="3" t="s">
         <v>306</v>
       </c>
       <c r="K86" s="0" t="s">
         <v>297</v>
       </c>
-      <c r="L86" s="1" t="n">
+      <c r="L86" s="4" t="n">
         <v>75</v>
       </c>
       <c r="N86" s="0" t="n">
@@ -4443,13 +4444,13 @@
       <c r="H87" s="0" t="s">
         <v>310</v>
       </c>
-      <c r="J87" s="4" t="s">
+      <c r="J87" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K87" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="L87" s="1" t="n">
+      <c r="L87" s="4" t="n">
         <v>0.6</v>
       </c>
       <c r="N87" s="0" t="n">
@@ -4472,13 +4473,13 @@
       <c r="H88" s="0" t="s">
         <v>313</v>
       </c>
-      <c r="J88" s="4" t="s">
+      <c r="J88" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K88" s="0" t="s">
         <v>311</v>
       </c>
-      <c r="L88" s="1" t="n">
+      <c r="L88" s="4" t="n">
         <v>0.3</v>
       </c>
       <c r="N88" s="0" t="n">
@@ -4501,13 +4502,13 @@
       <c r="H89" s="0" t="s">
         <v>315</v>
       </c>
-      <c r="J89" s="4" t="s">
+      <c r="J89" s="3" t="s">
         <v>316</v>
       </c>
       <c r="K89" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="L89" s="1" t="n">
+      <c r="L89" s="4" t="n">
         <v>0.7</v>
       </c>
       <c r="N89" s="0" t="n">
@@ -4530,10 +4531,10 @@
       <c r="H90" s="0" t="s">
         <v>319</v>
       </c>
-      <c r="J90" s="4" t="s">
+      <c r="J90" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L90" s="1" t="n">
+      <c r="L90" s="4" t="n">
         <v>0.6</v>
       </c>
       <c r="N90" s="0" t="n">
@@ -4556,13 +4557,13 @@
       <c r="H91" s="0" t="s">
         <v>321</v>
       </c>
-      <c r="J91" s="4" t="s">
+      <c r="J91" s="3" t="s">
         <v>52</v>
       </c>
       <c r="K91" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="L91" s="1" t="n">
+      <c r="L91" s="4" t="n">
         <v>1.2</v>
       </c>
       <c r="N91" s="0" t="n">
@@ -4585,13 +4586,13 @@
       <c r="H92" s="0" t="s">
         <v>323</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="J92" s="3" t="s">
         <v>324</v>
       </c>
       <c r="K92" s="0" t="s">
         <v>248</v>
       </c>
-      <c r="L92" s="1" t="n">
+      <c r="L92" s="4" t="n">
         <v>1.19</v>
       </c>
       <c r="N92" s="0" t="n">
@@ -4611,7 +4612,7 @@
       <c r="E93" s="0" t="s">
         <v>327</v>
       </c>
-      <c r="J93" s="4"/>
+      <c r="J93" s="3"/>
       <c r="N93" s="0" t="n">
         <v>0</v>
       </c>
@@ -4629,7 +4630,7 @@
       <c r="E94" s="0" t="s">
         <v>328</v>
       </c>
-      <c r="J94" s="4"/>
+      <c r="J94" s="3"/>
       <c r="N94" s="0" t="n">
         <v>0</v>
       </c>
@@ -4647,7 +4648,7 @@
       <c r="E95" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="J95" s="4"/>
+      <c r="J95" s="3"/>
       <c r="N95" s="0" t="n">
         <v>0</v>
       </c>
@@ -4665,7 +4666,7 @@
       <c r="E96" s="0" t="s">
         <v>330</v>
       </c>
-      <c r="J96" s="4"/>
+      <c r="J96" s="3"/>
       <c r="N96" s="0" t="n">
         <v>0</v>
       </c>
@@ -4683,7 +4684,7 @@
       <c r="E97" s="0" t="s">
         <v>331</v>
       </c>
-      <c r="J97" s="4"/>
+      <c r="J97" s="3"/>
       <c r="N97" s="0" t="n">
         <v>0</v>
       </c>
@@ -4701,7 +4702,7 @@
       <c r="E98" s="0" t="s">
         <v>332</v>
       </c>
-      <c r="J98" s="4"/>
+      <c r="J98" s="3"/>
       <c r="N98" s="0" t="n">
         <v>0</v>
       </c>
@@ -4719,7 +4720,7 @@
       <c r="E99" s="0" t="s">
         <v>333</v>
       </c>
-      <c r="J99" s="4"/>
+      <c r="J99" s="3"/>
       <c r="N99" s="0" t="n">
         <v>0</v>
       </c>
@@ -4737,7 +4738,7 @@
       <c r="E100" s="0" t="s">
         <v>329</v>
       </c>
-      <c r="J100" s="4"/>
+      <c r="J100" s="3"/>
       <c r="N100" s="0" t="n">
         <v>0</v>
       </c>
@@ -4755,7 +4756,7 @@
       <c r="E101" s="0" t="s">
         <v>335</v>
       </c>
-      <c r="J101" s="4"/>
+      <c r="J101" s="3"/>
       <c r="N101" s="0" t="n">
         <v>0</v>
       </c>
@@ -4814,28 +4815,28 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="1">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>338</v>
       </c>
     </row>
@@ -4849,10 +4850,10 @@
       <c r="C2" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>342</v>
       </c>
       <c r="F2" s="0" t="s">
@@ -4875,10 +4876,10 @@
       <c r="C3" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>345</v>
       </c>
       <c r="F3" s="0" t="s">
@@ -4901,10 +4902,10 @@
       <c r="C4" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>348</v>
       </c>
       <c r="F4" s="0" t="s">
@@ -4927,10 +4928,10 @@
       <c r="C5" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>351</v>
       </c>
       <c r="F5" s="0" t="s">
@@ -4953,10 +4954,10 @@
       <c r="C6" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>355</v>
       </c>
       <c r="F6" s="0" t="s">
@@ -4979,10 +4980,10 @@
       <c r="C7" s="0" t="s">
         <v>340</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="3" t="s">
         <v>358</v>
       </c>
       <c r="F7" s="0" t="s">
@@ -5005,10 +5006,10 @@
       <c r="C8" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>363</v>
       </c>
       <c r="F8" s="0" t="s">
@@ -5031,10 +5032,10 @@
       <c r="C9" s="0" t="s">
         <v>361</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>367</v>
       </c>
       <c r="F9" s="0" t="s">
@@ -5057,10 +5058,10 @@
       <c r="C10" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>370</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>370</v>
       </c>
       <c r="F10" s="0" t="s">
@@ -5083,10 +5084,10 @@
       <c r="C11" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>372</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="3" t="s">
         <v>372</v>
       </c>
       <c r="F11" s="0" t="s">
@@ -5109,10 +5110,10 @@
       <c r="C12" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>374</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="3" t="s">
         <v>374</v>
       </c>
       <c r="F12" s="0" t="s">
@@ -5135,10 +5136,10 @@
       <c r="C13" s="0" t="s">
         <v>369</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="3" t="s">
         <v>376</v>
       </c>
       <c r="F13" s="0" t="s">
@@ -5161,10 +5162,10 @@
       <c r="C14" s="0" t="s">
         <v>378</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="E14" s="3" t="s">
         <v>380</v>
       </c>
       <c r="F14" s="0" t="s">
@@ -5187,10 +5188,10 @@
       <c r="C15" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>383</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="3" t="s">
         <v>384</v>
       </c>
       <c r="F15" s="0" t="s">
@@ -5213,10 +5214,10 @@
       <c r="C16" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="E16" s="3" t="s">
         <v>388</v>
       </c>
       <c r="F16" s="0" t="s">
@@ -5239,10 +5240,10 @@
       <c r="C17" s="0" t="s">
         <v>382</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="3" t="s">
         <v>391</v>
       </c>
       <c r="F17" s="0" t="s">
@@ -5265,10 +5266,10 @@
       <c r="C18" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="3" t="s">
         <v>394</v>
       </c>
       <c r="F18" s="0" t="s">
@@ -5291,10 +5292,10 @@
       <c r="C19" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="3" t="s">
         <v>397</v>
       </c>
       <c r="F19" s="0" t="s">
@@ -5317,10 +5318,10 @@
       <c r="C20" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="3" t="s">
         <v>400</v>
       </c>
       <c r="F20" s="0" t="s">
@@ -5343,10 +5344,10 @@
       <c r="C21" s="0" t="s">
         <v>393</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="3" t="s">
         <v>402</v>
       </c>
       <c r="F21" s="0" t="s">
@@ -5369,10 +5370,10 @@
       <c r="C22" s="0" t="s">
         <v>404</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="3" t="s">
         <v>406</v>
       </c>
       <c r="F22" s="0" t="s">
@@ -5395,10 +5396,10 @@
       <c r="C23" s="0" t="s">
         <v>409</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F23" s="0" t="s">
@@ -5429,7 +5430,7 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B20" activeCellId="0" pane="topLeft" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -5448,37 +5449,37 @@
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="1" s="7">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>418</v>
       </c>
     </row>
@@ -6112,7 +6113,7 @@
         <v>504</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.2" outlineLevel="0" r="20">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.15" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>

</xml_diff>